<commit_message>
Adding proportions by trusts
</commit_message>
<xml_diff>
--- a/Code lists.xlsx
+++ b/Code lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/nhp_paeds_fracture_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1047" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA8C621-F4BD-44FE-9A2E-335659330CB8}"/>
+  <xr:revisionPtr revIDLastSave="1051" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4667611A-A080-4F1E-A247-2655C65F04F0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fracture codes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="414">
   <si>
     <t xml:space="preserve"> Fracture of clavicle</t>
   </si>
@@ -1275,13 +1275,19 @@
   </si>
   <si>
     <t>FOREARM</t>
+  </si>
+  <si>
+    <t>TO ADD</t>
+  </si>
+  <si>
+    <t>W663 Primary manipulative closed reduction of fracture dislocation of joint NEC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1345,6 +1351,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1478,7 +1490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1546,6 +1558,7 @@
     <xf numFmtId="1" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1970,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B350"/>
     </sheetView>
   </sheetViews>
@@ -5078,18 +5091,20 @@
   <conditionalFormatting sqref="A147:A1048576">
     <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="A1:E320 A321:C1048576 D322:E1048576">
+    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="12295008">
+      <formula>NOT(ISERROR(SEARCH("12295008",A1)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E320 D322:E1048576 A321:C1048576">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="12295008">
-      <formula>NOT(ISERROR(SEARCH("12295008",A1)))</formula>
-    </cfRule>
-    <cfRule type="duplicateValues" dxfId="2" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F320 D322:F1048576 A321:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5544,10 +5559,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6313E5DA-192A-4DE5-9440-CA22C3D70D8E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5625,6 +5640,14 @@
         <v>256</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="61" t="s">
+        <v>413</v>
+      </c>
+      <c r="D13" t="s">
+        <v>412</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated SQL and code lists
</commit_message>
<xml_diff>
--- a/Code lists.xlsx
+++ b/Code lists.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/nhp_paeds_fracture_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1051" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4667611A-A080-4F1E-A247-2655C65F04F0}"/>
+  <xr:revisionPtr revIDLastSave="1123" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2DF231-CFE2-45A0-89DB-726982CCDA92}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fracture codes" sheetId="1" r:id="rId1"/>
     <sheet name="ED codes" sheetId="3" r:id="rId2"/>
     <sheet name="Outpatient codes" sheetId="4" r:id="rId3"/>
     <sheet name="Inpatient codes" sheetId="5" r:id="rId4"/>
+    <sheet name="vs GIRFT" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="427">
   <si>
     <t xml:space="preserve"> Fracture of clavicle</t>
   </si>
@@ -1277,17 +1278,56 @@
     <t>FOREARM</t>
   </si>
   <si>
-    <t>TO ADD</t>
-  </si>
-  <si>
     <t>W663 Primary manipulative closed reduction of fracture dislocation of joint NEC</t>
+  </si>
+  <si>
+    <t>Our work</t>
+  </si>
+  <si>
+    <t>GIRFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only attendances at major A&amp;Es, excluded UTC/walk-in centres </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Wrist/Forearm manipulations in theatre per 10,000 A&amp;E attendances</t>
+  </si>
+  <si>
+    <t>Fractures</t>
+  </si>
+  <si>
+    <t>Attendances</t>
+  </si>
+  <si>
+    <t>Manipulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> W262, W268, W269, W663, included manipulation of fracture dislocation, but excluded re-manipulations and manipulation with skeletal traction</t>
+  </si>
+  <si>
+    <t>Snomed codes- All closed forearm/wrist fractures, excluded open /birth related/ pathological/ osteoporotic fractures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>W26, so includes re-manipulations and manipulation with skeletal traction. Plus W252 Closed reduction of fracture of bone and fixation using functional bracing system</t>
+  </si>
+  <si>
+    <t>ICD10- S52 Fracture of forearm and S62 Fracture of wrist. Includes open fractures</t>
+  </si>
+  <si>
+    <t>W252 Closed reduction of fracture of bone and fixation using functional bracing system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1357,6 +1397,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1490,7 +1538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1559,6 +1607,16 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5559,10 +5617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6313E5DA-192A-4DE5-9440-CA22C3D70D8E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5642,10 +5700,85 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="61" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3684A88-F092-44F5-A409-BBA17E353F49}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="63" t="s">
         <v>413</v>
       </c>
-      <c r="D13" t="s">
-        <v>412</v>
+      <c r="C1" s="63" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>421</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding code lists and methods
</commit_message>
<xml_diff>
--- a/Code lists.xlsx
+++ b/Code lists.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1123" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2DF231-CFE2-45A0-89DB-726982CCDA92}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="19812" windowHeight="13800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fracture codes" sheetId="1" r:id="rId1"/>
@@ -5174,7 +5174,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5327,8 +5327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1846D8A-3306-4A36-8870-7FE528F12F31}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5717,7 +5717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3684A88-F092-44F5-A409-BBA17E353F49}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to targets and functions
</commit_message>
<xml_diff>
--- a/Code lists.xlsx
+++ b/Code lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/nhp_paeds_fracture_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1123" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF2DF231-CFE2-45A0-89DB-726982CCDA92}"/>
+  <xr:revisionPtr revIDLastSave="1144" documentId="8_{5BDDECE6-181C-4155-BED5-868CDFF4BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42F93BB8-F1AB-4EB0-BE01-B1692E3C8D44}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="19812" windowHeight="13800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fracture codes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
   <si>
     <t xml:space="preserve"> Fracture of clavicle</t>
   </si>
@@ -1320,7 +1320,34 @@
     <t>ICD10- S52 Fracture of forearm and S62 Fracture of wrist. Includes open fractures</t>
   </si>
   <si>
-    <t>W252 Closed reduction of fracture of bone and fixation using functional bracing system</t>
+    <t>W25 Closed reduction of fracture of bone and external fixation</t>
+  </si>
+  <si>
+    <t>  Includes: External fixation of fracture of bone without mention of reduction</t>
+  </si>
+  <si>
+    <t>Excludes: Fracture dislocation (W66)</t>
+  </si>
+  <si>
+    <t>  Includes: Closed reduction of fracture of bone and fixation using cast brace</t>
+  </si>
+  <si>
+    <t>W251 Closed reduction of fracture of bone and fixation to skeleton HFQ</t>
+  </si>
+  <si>
+    <t>W252 Closed reduction of fracture of bone and fixation using functional bracing system</t>
+  </si>
+  <si>
+    <t>W253 Remanipulation of fracture of bone and external fixation HFQ </t>
+  </si>
+  <si>
+    <t>W258 Other specified</t>
+  </si>
+  <si>
+    <t>W259 Unspecified</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1617,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1606,7 +1632,6 @@
     <xf numFmtId="1" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1617,6 +1642,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3992,810 +4019,810 @@
       <c r="C218" s="28"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A220" s="51" t="s">
+      <c r="A220" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="B220" s="52"/>
-      <c r="C220" s="53"/>
+      <c r="B220" s="51"/>
+      <c r="C220" s="52"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A221" s="54">
+      <c r="A221" s="53">
         <v>31978002</v>
       </c>
-      <c r="B221" s="55" t="s">
+      <c r="B221" s="54" t="s">
         <v>327</v>
       </c>
-      <c r="C221" s="50"/>
+      <c r="C221" s="49"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A222" s="48">
+      <c r="A222" s="47">
         <v>6698000</v>
       </c>
-      <c r="B222" s="49" t="s">
+      <c r="B222" s="48" t="s">
         <v>265</v>
       </c>
-      <c r="C222" s="50"/>
+      <c r="C222" s="49"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A223" s="48">
+      <c r="A223" s="47">
         <v>6990005</v>
       </c>
-      <c r="B223" s="49" t="s">
+      <c r="B223" s="48" t="s">
         <v>266</v>
       </c>
-      <c r="C223" s="50"/>
+      <c r="C223" s="49"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A224" s="48">
+      <c r="A224" s="47">
         <v>15385006</v>
       </c>
-      <c r="B224" s="49" t="s">
+      <c r="B224" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="C224" s="50"/>
+      <c r="C224" s="49"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A225" s="48">
+      <c r="A225" s="47">
         <v>20433007</v>
       </c>
-      <c r="B225" s="49" t="s">
+      <c r="B225" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="C225" s="50"/>
+      <c r="C225" s="49"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A226" s="48">
+      <c r="A226" s="47">
         <v>23900009</v>
       </c>
-      <c r="B226" s="49" t="s">
+      <c r="B226" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="C226" s="50"/>
+      <c r="C226" s="49"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A227" s="48">
+      <c r="A227" s="47">
         <v>25899002</v>
       </c>
-      <c r="B227" s="49" t="s">
+      <c r="B227" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="C227" s="50"/>
+      <c r="C227" s="49"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A228" s="48">
+      <c r="A228" s="47">
         <v>28012007</v>
       </c>
-      <c r="B228" s="49" t="s">
+      <c r="B228" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="C228" s="50"/>
+      <c r="C228" s="49"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A229" s="48">
+      <c r="A229" s="47">
         <v>47848000</v>
       </c>
-      <c r="B229" s="49" t="s">
+      <c r="B229" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="C229" s="50"/>
+      <c r="C229" s="49"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A230" s="48">
+      <c r="A230" s="47">
         <v>71830006</v>
       </c>
-      <c r="B230" s="49" t="s">
+      <c r="B230" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="C230" s="50"/>
+      <c r="C230" s="49"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A231" s="48">
+      <c r="A231" s="47">
         <v>87905008</v>
       </c>
-      <c r="B231" s="49" t="s">
+      <c r="B231" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="C231" s="50"/>
+      <c r="C231" s="49"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A232" s="48">
+      <c r="A232" s="47">
         <v>123975002</v>
       </c>
-      <c r="B232" s="49" t="s">
+      <c r="B232" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="C232" s="50"/>
+      <c r="C232" s="49"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A233" s="48">
+      <c r="A233" s="47">
         <v>208610006</v>
       </c>
-      <c r="B233" s="49" t="s">
+      <c r="B233" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="C233" s="50"/>
+      <c r="C233" s="49"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A234" s="48">
+      <c r="A234" s="47">
         <v>208611005</v>
       </c>
-      <c r="B234" s="49" t="s">
+      <c r="B234" s="48" t="s">
         <v>277</v>
       </c>
-      <c r="C234" s="50"/>
+      <c r="C234" s="49"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A235" s="48">
+      <c r="A235" s="47">
         <v>208612003</v>
       </c>
-      <c r="B235" s="49" t="s">
+      <c r="B235" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="C235" s="50"/>
+      <c r="C235" s="49"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A236" s="48">
+      <c r="A236" s="47">
         <v>208613008</v>
       </c>
-      <c r="B236" s="49" t="s">
+      <c r="B236" s="48" t="s">
         <v>279</v>
       </c>
-      <c r="C236" s="50"/>
+      <c r="C236" s="49"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A237" s="48">
+      <c r="A237" s="47">
         <v>208629000</v>
       </c>
-      <c r="B237" s="49" t="s">
+      <c r="B237" s="48" t="s">
         <v>280</v>
       </c>
-      <c r="C237" s="50"/>
+      <c r="C237" s="49"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A238" s="48">
+      <c r="A238" s="47">
         <v>208634001</v>
       </c>
-      <c r="B238" s="49" t="s">
+      <c r="B238" s="48" t="s">
         <v>281</v>
       </c>
-      <c r="C238" s="50"/>
+      <c r="C238" s="49"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A239" s="48">
+      <c r="A239" s="47">
         <v>208635000</v>
       </c>
-      <c r="B239" s="49" t="s">
+      <c r="B239" s="48" t="s">
         <v>282</v>
       </c>
-      <c r="C239" s="50"/>
+      <c r="C239" s="49"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A240" s="48">
+      <c r="A240" s="47">
         <v>208636004</v>
       </c>
-      <c r="B240" s="49" t="s">
+      <c r="B240" s="48" t="s">
         <v>283</v>
       </c>
-      <c r="C240" s="50"/>
+      <c r="C240" s="49"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A241" s="48">
+      <c r="A241" s="47">
         <v>208662008</v>
       </c>
-      <c r="B241" s="49" t="s">
+      <c r="B241" s="48" t="s">
         <v>284</v>
       </c>
-      <c r="C241" s="50"/>
+      <c r="C241" s="49"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A242" s="48">
+      <c r="A242" s="47">
         <v>208663003</v>
       </c>
-      <c r="B242" s="49" t="s">
+      <c r="B242" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="C242" s="50"/>
+      <c r="C242" s="49"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A243" s="48">
+      <c r="A243" s="47">
         <v>208666006</v>
       </c>
-      <c r="B243" s="49" t="s">
+      <c r="B243" s="48" t="s">
         <v>286</v>
       </c>
-      <c r="C243" s="50"/>
+      <c r="C243" s="49"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A244" s="48">
+      <c r="A244" s="47">
         <v>208667002</v>
       </c>
-      <c r="B244" s="49" t="s">
+      <c r="B244" s="48" t="s">
         <v>287</v>
       </c>
-      <c r="C244" s="50"/>
+      <c r="C244" s="49"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A245" s="48">
+      <c r="A245" s="47">
         <v>263237009</v>
       </c>
-      <c r="B245" s="49" t="s">
+      <c r="B245" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="C245" s="50"/>
+      <c r="C245" s="49"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A246" s="48">
+      <c r="A246" s="47">
         <v>263240009</v>
       </c>
-      <c r="B246" s="49" t="s">
+      <c r="B246" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="C246" s="50"/>
+      <c r="C246" s="49"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A247" s="48">
+      <c r="A247" s="47">
         <v>263241008</v>
       </c>
-      <c r="B247" s="49" t="s">
+      <c r="B247" s="48" t="s">
         <v>290</v>
       </c>
-      <c r="C247" s="50"/>
+      <c r="C247" s="49"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A248" s="48">
+      <c r="A248" s="47">
         <v>263244000</v>
       </c>
-      <c r="B248" s="49" t="s">
+      <c r="B248" s="48" t="s">
         <v>291</v>
       </c>
-      <c r="C248" s="50"/>
+      <c r="C248" s="49"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A249" s="48">
+      <c r="A249" s="47">
         <v>271577005</v>
       </c>
-      <c r="B249" s="49" t="s">
+      <c r="B249" s="48" t="s">
         <v>292</v>
       </c>
-      <c r="C249" s="50"/>
+      <c r="C249" s="49"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A250" s="48">
+      <c r="A250" s="47">
         <v>278537006</v>
       </c>
-      <c r="B250" s="49" t="s">
+      <c r="B250" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="C250" s="50"/>
+      <c r="C250" s="49"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A251" s="48">
+      <c r="A251" s="47">
         <v>281531008</v>
       </c>
-      <c r="B251" s="49" t="s">
+      <c r="B251" s="48" t="s">
         <v>294</v>
       </c>
-      <c r="C251" s="50"/>
+      <c r="C251" s="49"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A252" s="48">
+      <c r="A252" s="47">
         <v>281532001</v>
       </c>
-      <c r="B252" s="49" t="s">
+      <c r="B252" s="48" t="s">
         <v>295</v>
       </c>
-      <c r="C252" s="50"/>
+      <c r="C252" s="49"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A253" s="48">
+      <c r="A253" s="47">
         <v>281843000</v>
       </c>
-      <c r="B253" s="49" t="s">
+      <c r="B253" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="C253" s="50"/>
+      <c r="C253" s="49"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A254" s="48">
+      <c r="A254" s="47">
         <v>413877007</v>
       </c>
-      <c r="B254" s="49" t="s">
+      <c r="B254" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="C254" s="50"/>
+      <c r="C254" s="49"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A255" s="48">
+      <c r="A255" s="47">
         <v>414293001</v>
       </c>
-      <c r="B255" s="49" t="s">
+      <c r="B255" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="C255" s="50"/>
+      <c r="C255" s="49"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A256" s="48">
+      <c r="A256" s="47">
         <v>428256003</v>
       </c>
-      <c r="B256" s="49" t="s">
+      <c r="B256" s="48" t="s">
         <v>299</v>
       </c>
-      <c r="C256" s="50"/>
+      <c r="C256" s="49"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A257" s="48">
+      <c r="A257" s="47">
         <v>428257007</v>
       </c>
-      <c r="B257" s="49" t="s">
+      <c r="B257" s="48" t="s">
         <v>300</v>
       </c>
-      <c r="C257" s="50"/>
+      <c r="C257" s="49"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A258" s="48">
+      <c r="A258" s="47">
         <v>428797006</v>
       </c>
-      <c r="B258" s="49" t="s">
+      <c r="B258" s="48" t="s">
         <v>301</v>
       </c>
-      <c r="C258" s="50"/>
+      <c r="C258" s="49"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A259" s="48">
+      <c r="A259" s="47">
         <v>428798001</v>
       </c>
-      <c r="B259" s="49" t="s">
+      <c r="B259" s="48" t="s">
         <v>302</v>
       </c>
-      <c r="C259" s="50"/>
+      <c r="C259" s="49"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A260" s="48">
+      <c r="A260" s="47">
         <v>442205007</v>
       </c>
-      <c r="B260" s="49" t="s">
+      <c r="B260" s="48" t="s">
         <v>303</v>
       </c>
-      <c r="C260" s="50"/>
+      <c r="C260" s="49"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A261" s="48">
+      <c r="A261" s="47">
         <v>445410003</v>
       </c>
-      <c r="B261" s="49" t="s">
+      <c r="B261" s="48" t="s">
         <v>304</v>
       </c>
-      <c r="C261" s="50"/>
+      <c r="C261" s="49"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A262" s="48">
+      <c r="A262" s="47">
         <v>446298003</v>
       </c>
-      <c r="B262" s="49" t="s">
+      <c r="B262" s="48" t="s">
         <v>305</v>
       </c>
-      <c r="C262" s="50"/>
+      <c r="C262" s="49"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A263" s="48">
+      <c r="A263" s="47">
         <v>447139008</v>
       </c>
-      <c r="B263" s="49" t="s">
+      <c r="B263" s="48" t="s">
         <v>306</v>
       </c>
-      <c r="C263" s="50"/>
+      <c r="C263" s="49"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A264" s="48">
+      <c r="A264" s="47">
         <v>703998005</v>
       </c>
-      <c r="B264" s="49" t="s">
+      <c r="B264" s="48" t="s">
         <v>307</v>
       </c>
-      <c r="C264" s="50"/>
+      <c r="C264" s="49"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A265" s="48">
+      <c r="A265" s="47">
         <v>705080006</v>
       </c>
-      <c r="B265" s="49" t="s">
+      <c r="B265" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="C265" s="50"/>
+      <c r="C265" s="49"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A266" s="48">
+      <c r="A266" s="47">
         <v>705092006</v>
       </c>
-      <c r="B266" s="49" t="s">
+      <c r="B266" s="48" t="s">
         <v>309</v>
       </c>
-      <c r="C266" s="50"/>
+      <c r="C266" s="49"/>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A267" s="48">
+      <c r="A267" s="47">
         <v>733295004</v>
       </c>
-      <c r="B267" s="49" t="s">
+      <c r="B267" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="C267" s="50"/>
+      <c r="C267" s="49"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A268" s="48">
+      <c r="A268" s="47">
         <v>735669008</v>
       </c>
-      <c r="B268" s="49" t="s">
+      <c r="B268" s="48" t="s">
         <v>311</v>
       </c>
-      <c r="C268" s="50"/>
+      <c r="C268" s="49"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A269" s="48">
+      <c r="A269" s="47">
         <v>735671008</v>
       </c>
-      <c r="B269" s="49" t="s">
+      <c r="B269" s="48" t="s">
         <v>312</v>
       </c>
-      <c r="C269" s="50"/>
+      <c r="C269" s="49"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A270" s="48">
+      <c r="A270" s="47">
         <v>735672001</v>
       </c>
-      <c r="B270" s="49" t="s">
+      <c r="B270" s="48" t="s">
         <v>313</v>
       </c>
-      <c r="C270" s="50"/>
+      <c r="C270" s="49"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A271" s="48">
+      <c r="A271" s="47">
         <v>735846008</v>
       </c>
-      <c r="B271" s="49" t="s">
+      <c r="B271" s="48" t="s">
         <v>314</v>
       </c>
-      <c r="C271" s="50"/>
+      <c r="C271" s="49"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A272" s="48">
+      <c r="A272" s="47">
         <v>39541000087106</v>
       </c>
-      <c r="B272" s="49" t="s">
+      <c r="B272" s="48" t="s">
         <v>315</v>
       </c>
-      <c r="C272" s="50"/>
+      <c r="C272" s="49"/>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A273" s="48">
+      <c r="A273" s="47">
         <v>39551000087109</v>
       </c>
-      <c r="B273" s="49" t="s">
+      <c r="B273" s="48" t="s">
         <v>316</v>
       </c>
-      <c r="C273" s="50"/>
+      <c r="C273" s="49"/>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A274" s="48">
+      <c r="A274" s="47">
         <v>40031000087104</v>
       </c>
-      <c r="B274" s="49" t="s">
+      <c r="B274" s="48" t="s">
         <v>317</v>
       </c>
-      <c r="C274" s="50"/>
+      <c r="C274" s="49"/>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A275" s="48">
+      <c r="A275" s="47">
         <v>40041000087105</v>
       </c>
-      <c r="B275" s="49" t="s">
+      <c r="B275" s="48" t="s">
         <v>318</v>
       </c>
-      <c r="C275" s="50"/>
+      <c r="C275" s="49"/>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A276" s="48">
+      <c r="A276" s="47">
         <v>40051000087108</v>
       </c>
-      <c r="B276" s="49" t="s">
+      <c r="B276" s="48" t="s">
         <v>319</v>
       </c>
-      <c r="C276" s="50"/>
+      <c r="C276" s="49"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A277" s="48">
+      <c r="A277" s="47">
         <v>40061000087106</v>
       </c>
-      <c r="B277" s="49" t="s">
+      <c r="B277" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="C277" s="50"/>
+      <c r="C277" s="49"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A278" s="48">
+      <c r="A278" s="47">
         <v>40071000087102</v>
       </c>
-      <c r="B278" s="49" t="s">
+      <c r="B278" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="C278" s="50"/>
+      <c r="C278" s="49"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A279" s="48">
+      <c r="A279" s="47">
         <v>40081000087100</v>
       </c>
-      <c r="B279" s="49" t="s">
+      <c r="B279" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="C279" s="50"/>
+      <c r="C279" s="49"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A280" s="48">
+      <c r="A280" s="47">
         <v>1.09248410001191E+16</v>
       </c>
-      <c r="B280" s="49" t="s">
+      <c r="B280" s="48" t="s">
         <v>323</v>
       </c>
-      <c r="C280" s="50"/>
+      <c r="C280" s="49"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A281" s="48">
+      <c r="A281" s="47">
         <v>1.09248810001191E+16</v>
       </c>
-      <c r="B281" s="49" t="s">
+      <c r="B281" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="C281" s="50"/>
+      <c r="C281" s="49"/>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A282" s="54">
+      <c r="A282" s="53">
         <v>75591007</v>
       </c>
-      <c r="B282" s="55" t="s">
+      <c r="B282" s="54" t="s">
         <v>328</v>
       </c>
-      <c r="C282" s="50"/>
+      <c r="C282" s="49"/>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A283" s="54">
+      <c r="A283" s="53">
         <v>21867001</v>
       </c>
-      <c r="B283" s="55" t="s">
+      <c r="B283" s="54" t="s">
         <v>329</v>
       </c>
-      <c r="C283" s="50"/>
+      <c r="C283" s="49"/>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A284" s="54">
+      <c r="A284" s="53">
         <v>28359007</v>
       </c>
-      <c r="B284" s="55" t="s">
+      <c r="B284" s="54" t="s">
         <v>330</v>
       </c>
-      <c r="C284" s="50"/>
+      <c r="C284" s="49"/>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A285" s="54">
+      <c r="A285" s="53">
         <v>34268009</v>
       </c>
-      <c r="B285" s="55" t="s">
+      <c r="B285" s="54" t="s">
         <v>331</v>
       </c>
-      <c r="C285" s="50"/>
+      <c r="C285" s="49"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A286" s="54">
+      <c r="A286" s="53">
         <v>59639009</v>
       </c>
-      <c r="B286" s="55" t="s">
+      <c r="B286" s="54" t="s">
         <v>332</v>
       </c>
-      <c r="C286" s="50"/>
+      <c r="C286" s="49"/>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A287" s="54">
+      <c r="A287" s="53">
         <v>67394003</v>
       </c>
-      <c r="B287" s="55" t="s">
+      <c r="B287" s="54" t="s">
         <v>333</v>
       </c>
-      <c r="C287" s="50"/>
+      <c r="C287" s="49"/>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A288" s="54">
+      <c r="A288" s="53">
         <v>77803008</v>
       </c>
-      <c r="B288" s="55" t="s">
+      <c r="B288" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C288" s="50"/>
+      <c r="C288" s="49"/>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A289" s="54">
+      <c r="A289" s="53">
         <v>208615001</v>
       </c>
-      <c r="B289" s="55" t="s">
+      <c r="B289" s="54" t="s">
         <v>335</v>
       </c>
-      <c r="C289" s="50"/>
+      <c r="C289" s="49"/>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A290" s="54">
+      <c r="A290" s="53">
         <v>208657007</v>
       </c>
-      <c r="B290" s="55" t="s">
+      <c r="B290" s="54" t="s">
         <v>336</v>
       </c>
-      <c r="C290" s="50"/>
+      <c r="C290" s="49"/>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A291" s="54">
+      <c r="A291" s="53">
         <v>208658002</v>
       </c>
-      <c r="B291" s="55" t="s">
+      <c r="B291" s="54" t="s">
         <v>337</v>
       </c>
-      <c r="C291" s="50"/>
+      <c r="C291" s="49"/>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A292" s="54">
+      <c r="A292" s="53">
         <v>263242001</v>
       </c>
-      <c r="B292" s="55" t="s">
+      <c r="B292" s="54" t="s">
         <v>338</v>
       </c>
-      <c r="C292" s="50"/>
+      <c r="C292" s="49"/>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A293" s="54">
+      <c r="A293" s="53">
         <v>281533006</v>
       </c>
-      <c r="B293" s="55" t="s">
+      <c r="B293" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="C293" s="50"/>
+      <c r="C293" s="49"/>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A294" s="54">
+      <c r="A294" s="53">
         <v>281534000</v>
       </c>
-      <c r="B294" s="55" t="s">
+      <c r="B294" s="54" t="s">
         <v>340</v>
       </c>
-      <c r="C294" s="50"/>
+      <c r="C294" s="49"/>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A295" s="54">
+      <c r="A295" s="53">
         <v>281535004</v>
       </c>
-      <c r="B295" s="55" t="s">
+      <c r="B295" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="C295" s="50"/>
+      <c r="C295" s="49"/>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A296" s="54">
+      <c r="A296" s="53">
         <v>308153009</v>
       </c>
-      <c r="B296" s="55" t="s">
+      <c r="B296" s="54" t="s">
         <v>342</v>
       </c>
-      <c r="C296" s="50"/>
+      <c r="C296" s="49"/>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A297" s="54">
+      <c r="A297" s="53">
         <v>315643003</v>
       </c>
-      <c r="B297" s="55" t="s">
+      <c r="B297" s="54" t="s">
         <v>343</v>
       </c>
-      <c r="C297" s="50"/>
+      <c r="C297" s="49"/>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A298" s="54">
+      <c r="A298" s="53">
         <v>442538002</v>
       </c>
-      <c r="B298" s="55" t="s">
+      <c r="B298" s="54" t="s">
         <v>344</v>
       </c>
-      <c r="C298" s="50"/>
+      <c r="C298" s="49"/>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A299" s="54">
+      <c r="A299" s="53">
         <v>447395005</v>
       </c>
-      <c r="B299" s="55" t="s">
+      <c r="B299" s="54" t="s">
         <v>345</v>
       </c>
-      <c r="C299" s="50"/>
+      <c r="C299" s="49"/>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A300" s="54">
+      <c r="A300" s="53">
         <v>704209008</v>
       </c>
-      <c r="B300" s="55" t="s">
+      <c r="B300" s="54" t="s">
         <v>346</v>
       </c>
-      <c r="C300" s="50"/>
+      <c r="C300" s="49"/>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A301" s="54">
+      <c r="A301" s="53">
         <v>705082003</v>
       </c>
-      <c r="B301" s="55" t="s">
+      <c r="B301" s="54" t="s">
         <v>347</v>
       </c>
-      <c r="C301" s="50"/>
+      <c r="C301" s="49"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A302" s="54">
+      <c r="A302" s="53">
         <v>733296003</v>
       </c>
-      <c r="B302" s="55" t="s">
+      <c r="B302" s="54" t="s">
         <v>348</v>
       </c>
-      <c r="C302" s="50"/>
+      <c r="C302" s="49"/>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A303" s="54">
+      <c r="A303" s="53">
         <v>735842005</v>
       </c>
-      <c r="B303" s="55" t="s">
+      <c r="B303" s="54" t="s">
         <v>349</v>
       </c>
-      <c r="C303" s="50"/>
+      <c r="C303" s="49"/>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A304" s="54">
+      <c r="A304" s="53">
         <v>735844006</v>
       </c>
-      <c r="B304" s="55" t="s">
+      <c r="B304" s="54" t="s">
         <v>350</v>
       </c>
-      <c r="C304" s="50"/>
+      <c r="C304" s="49"/>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A305" s="54">
+      <c r="A305" s="53">
         <v>735845007</v>
       </c>
-      <c r="B305" s="55" t="s">
+      <c r="B305" s="54" t="s">
         <v>351</v>
       </c>
-      <c r="C305" s="50"/>
+      <c r="C305" s="49"/>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A306" s="54">
+      <c r="A306" s="53">
         <v>735847004</v>
       </c>
-      <c r="B306" s="55" t="s">
+      <c r="B306" s="54" t="s">
         <v>352</v>
       </c>
-      <c r="C306" s="50"/>
+      <c r="C306" s="49"/>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A307" s="54">
+      <c r="A307" s="53">
         <v>736517000</v>
       </c>
-      <c r="B307" s="55" t="s">
+      <c r="B307" s="54" t="s">
         <v>353</v>
       </c>
-      <c r="C307" s="50"/>
+      <c r="C307" s="49"/>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A308" s="54">
+      <c r="A308" s="53">
         <v>1.93500010000041E+16</v>
       </c>
-      <c r="B308" s="55" t="s">
+      <c r="B308" s="54" t="s">
         <v>325</v>
       </c>
-      <c r="C308" s="50"/>
+      <c r="C308" s="49"/>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A310" s="58" t="s">
+      <c r="A310" s="57" t="s">
         <v>411</v>
       </c>
-      <c r="B310" s="59"/>
-      <c r="C310" s="60"/>
+      <c r="B310" s="58"/>
+      <c r="C310" s="59"/>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" s="8">
@@ -5181,14 +5208,14 @@
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="101.21875" style="30" customWidth="1"/>
-    <col min="4" max="4" width="25" style="46" customWidth="1"/>
+    <col min="4" max="4" width="25" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>264</v>
       </c>
     </row>
@@ -5327,7 +5354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1846D8A-3306-4A36-8870-7FE528F12F31}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
@@ -5352,10 +5379,10 @@
       <c r="B2" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="D2" s="56">
+      <c r="D2" s="55">
         <v>1</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>354</v>
       </c>
       <c r="F2">
@@ -5369,10 +5396,10 @@
       <c r="B3" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="55">
         <v>2</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="55" t="s">
         <v>355</v>
       </c>
       <c r="F3">
@@ -5386,10 +5413,10 @@
       <c r="B4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="56">
         <v>10</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="56" t="s">
         <v>356</v>
       </c>
       <c r="F4">
@@ -5413,10 +5440,10 @@
       <c r="A6" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="55">
         <v>3</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="55" t="s">
         <v>358</v>
       </c>
       <c r="F6">
@@ -5430,10 +5457,10 @@
       <c r="B7" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="55">
         <v>92</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="55" t="s">
         <v>359</v>
       </c>
       <c r="F7">
@@ -5447,10 +5474,10 @@
       <c r="B8" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="55">
         <v>12</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="55" t="s">
         <v>360</v>
       </c>
       <c r="F8">
@@ -5464,10 +5491,10 @@
       <c r="B9" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="56">
         <v>4</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="56" t="s">
         <v>361</v>
       </c>
       <c r="F9">
@@ -5498,10 +5525,10 @@
       <c r="B11" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="55">
         <v>6</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="55" t="s">
         <v>363</v>
       </c>
       <c r="F11">
@@ -5515,10 +5542,10 @@
       <c r="B12" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="55">
         <v>7</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="55" t="s">
         <v>364</v>
       </c>
       <c r="F12">
@@ -5526,10 +5553,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="56">
+      <c r="D13" s="55">
         <v>13</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="55" t="s">
         <v>365</v>
       </c>
       <c r="F13">
@@ -5537,10 +5564,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="56">
+      <c r="D14" s="55">
         <v>14</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="55" t="s">
         <v>366</v>
       </c>
       <c r="F14">
@@ -5548,10 +5575,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="56">
+      <c r="D15" s="55">
         <v>15</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="55" t="s">
         <v>367</v>
       </c>
       <c r="F15">
@@ -5559,10 +5586,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="56">
+      <c r="D16" s="55">
         <v>16</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="55" t="s">
         <v>368</v>
       </c>
       <c r="F16">
@@ -5570,10 +5597,10 @@
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="56">
+      <c r="D17" s="55">
         <v>17</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="55" t="s">
         <v>369</v>
       </c>
       <c r="F17">
@@ -5581,10 +5608,10 @@
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="56">
+      <c r="D18" s="55">
         <v>93</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="55" t="s">
         <v>370</v>
       </c>
       <c r="F18">
@@ -5603,7 +5630,7 @@
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="55" t="s">
         <v>372</v>
       </c>
       <c r="F20">
@@ -5617,23 +5644,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6313E5DA-192A-4DE5-9440-CA22C3D70D8E}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="65" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="45"/>
+      <c r="B1" s="65"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5699,17 +5726,70 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="64" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B13" s="44"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>430</v>
+      </c>
+      <c r="C20" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="44" t="s">
+        <v>431</v>
+      </c>
+      <c r="B21" s="44"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="44" t="s">
+        <v>429</v>
+      </c>
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="43" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>433</v>
+      </c>
+      <c r="C24" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C25" t="s">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5724,33 +5804,33 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.88671875" customWidth="1"/>
-    <col min="2" max="2" width="54.44140625" style="62" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="62" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" style="60" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="61" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="61" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="62" t="s">
         <v>417</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>418</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="60" t="s">
         <v>422</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="60" t="s">
         <v>425</v>
       </c>
     </row>
@@ -5758,10 +5838,10 @@
       <c r="A4" t="s">
         <v>419</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="60" t="s">
         <v>415</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="60" t="s">
         <v>416</v>
       </c>
     </row>
@@ -5769,10 +5849,10 @@
       <c r="A5" t="s">
         <v>420</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="60" t="s">
         <v>421</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="60" t="s">
         <v>424</v>
       </c>
     </row>

</xml_diff>